<commit_message>
Últimas correciones de la Presentación + Preguntas
</commit_message>
<xml_diff>
--- a/Commits.xlsx
+++ b/Commits.xlsx
@@ -1,32 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFG\TFG_Microservices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAFFBF0-06A7-43CD-B2CE-FE7F8E74D516}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A0B048-FABA-4055-97C3-37321358A823}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{32396625-9C51-4A5C-869A-62AE6FBE7DC6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2" xr2:uid="{32396625-9C51-4A5C-869A-62AE6FBE7DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Commits" sheetId="1" r:id="rId1"/>
     <sheet name="Cronograma" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Solución monolítica</t>
   </si>
@@ -125,6 +131,30 @@
   </si>
   <si>
     <t>Adaptación de la interfaz de usuario</t>
+  </si>
+  <si>
+    <t>Microservicio</t>
+  </si>
+  <si>
+    <t>Implementación en el sist. monolítico</t>
+  </si>
+  <si>
+    <t>Refactorización en un microservicio</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>Informes</t>
+  </si>
+  <si>
+    <t>Notificaciones</t>
+  </si>
+  <si>
+    <t>Incidencias</t>
+  </si>
+  <si>
+    <t>Pedidos</t>
   </si>
 </sst>
 </file>
@@ -3707,6 +3737,384 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Implementación en el sist. monolítico</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$B$4:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Seguridad</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Informes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Notificaciones</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Incidencias</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Pedidos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$4:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D6F9-4333-86EF-2B04D30EF466}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Refactorización en un microservicio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$B$4:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Seguridad</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Informes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Notificaciones</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Incidencias</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Pedidos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D6F9-4333-86EF-2B04D30EF466}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="508895136"/>
+        <c:axId val="508896776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="508895136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508896776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="508896776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508895136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3827,6 +4235,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5332,6 +5780,511 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5410,15 +6363,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5476,6 +6429,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D04C1D-A6AB-4A04-BA2F-471943CBA07B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6504,8 +7498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8834853F-891F-4E9F-BC63-AFE8BC063A19}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7542,4 +8536,121 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B894A7C-1CCE-40CA-B91B-2506DB2D9ED8}">
+  <dimension ref="B3:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.88671875" customWidth="1"/>
+    <col min="11" max="11" width="30.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>SUM(C4:D4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E8" si="0">SUM(C5:D5)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="4">
+        <f>SUM(E4:E8)/5</f>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>